<commit_message>
CCS files from US version, remove outdated fuel file
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Calculations.xlsx
+++ b/InputData/ccs/CC/CCS Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathaniyer/Library/Containers/com.microsoft.Excel/Data/state-eps-data-repository/MN/ccs/CC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E15BAF0-09AB-984A-8355-524D564400A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715DE207-3FDF-46D8-8287-2B3597E1EC55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="147">
   <si>
     <t>Source:</t>
   </si>
@@ -883,9 +883,6 @@
   </si>
   <si>
     <t>Transportation and Storage Costs ($/tCO2)</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
   </si>
 </sst>
 </file>
@@ -1523,36 +1520,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" customWidth="1"/>
-    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1560,95 +1554,95 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="40">
         <v>2021</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="58" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="59">
         <v>0.97</v>
       </c>
@@ -1656,7 +1650,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
     </row>
   </sheetData>
@@ -1669,17 +1663,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A09EAE-4F9C-4AA7-B5E7-0962DD219D21}">
   <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>30</v>
       </c>
@@ -1691,7 +1685,7 @@
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
         <v>31</v>
@@ -1715,7 +1709,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>38</v>
       </c>
@@ -1741,7 +1735,7 @@
         <v>4286</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>86</v>
       </c>
@@ -1767,7 +1761,7 @@
         <v>4718</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>40</v>
       </c>
@@ -1793,7 +1787,7 @@
         <v>6133</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>41</v>
       </c>
@@ -1819,7 +1813,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>44</v>
       </c>
@@ -1845,7 +1839,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>46</v>
       </c>
@@ -1871,7 +1865,7 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>48</v>
       </c>
@@ -1897,7 +1891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>50</v>
       </c>
@@ -1923,7 +1917,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>55</v>
       </c>
@@ -1935,7 +1929,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>56</v>
       </c>
@@ -1947,7 +1941,7 @@
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>57</v>
       </c>
@@ -1973,7 +1967,7 @@
         <v>7446</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>59</v>
       </c>
@@ -1999,7 +1993,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>60</v>
       </c>
@@ -2025,7 +2019,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>61</v>
       </c>
@@ -2047,7 +2041,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>66</v>
       </c>
@@ -2073,7 +2067,7 @@
         <v>11.06</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>68</v>
       </c>
@@ -2099,7 +2093,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>70</v>
       </c>
@@ -2125,7 +2119,7 @@
         <v>9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>71</v>
       </c>
@@ -2151,7 +2145,7 @@
         <v>0.10970000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>72</v>
       </c>
@@ -2177,7 +2171,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>90</v>
       </c>
@@ -2203,7 +2197,7 @@
         <v>0.13969999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>73</v>
       </c>
@@ -2229,7 +2223,7 @@
         <v>9.2399999999999996E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>74</v>
       </c>
@@ -2253,7 +2247,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>75</v>
       </c>
@@ -2269,7 +2263,7 @@
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="21" t="s">
         <v>31</v>
@@ -2299,7 +2293,7 @@
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="51" t="s">
         <v>101</v>
       </c>
@@ -2323,7 +2317,7 @@
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>86</v>
       </c>
@@ -2347,7 +2341,7 @@
       <c r="K29" s="17"/>
       <c r="L29" s="17"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>102</v>
       </c>
@@ -2377,7 +2371,7 @@
       <c r="K30" s="17"/>
       <c r="L30" s="17"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>103</v>
       </c>
@@ -2407,7 +2401,7 @@
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>104</v>
       </c>
@@ -2439,7 +2433,7 @@
       <c r="L32" s="17"/>
       <c r="Y32" s="36"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>106</v>
       </c>
@@ -2471,7 +2465,7 @@
       <c r="L33" s="17"/>
       <c r="Y33" s="37"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>107</v>
       </c>
@@ -2502,7 +2496,7 @@
       <c r="J34" s="40"/>
       <c r="L34" s="17"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>109</v>
       </c>
@@ -2534,7 +2528,7 @@
       <c r="L35" s="17"/>
       <c r="Y35" s="35"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>110</v>
       </c>
@@ -2554,7 +2548,7 @@
       </c>
       <c r="J36" s="40"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="52" t="s">
         <v>111</v>
       </c>
@@ -2574,7 +2568,7 @@
       </c>
       <c r="J37" s="40"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>85</v>
       </c>
@@ -2611,7 +2605,7 @@
       </c>
       <c r="J38" s="40"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>113</v>
       </c>
@@ -2641,7 +2635,7 @@
       </c>
       <c r="J39" s="40"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>114</v>
       </c>
@@ -2671,7 +2665,7 @@
       </c>
       <c r="J40" s="40"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>115</v>
       </c>
@@ -2701,7 +2695,7 @@
       </c>
       <c r="J41" s="40"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>116</v>
       </c>
@@ -2731,7 +2725,7 @@
       </c>
       <c r="J42" s="40"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>118</v>
       </c>
@@ -2761,7 +2755,7 @@
       </c>
       <c r="J43" s="40"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>120</v>
       </c>
@@ -2791,7 +2785,7 @@
       </c>
       <c r="J44" s="40"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>121</v>
       </c>
@@ -2821,7 +2815,7 @@
       </c>
       <c r="J45" s="40"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>122</v>
       </c>
@@ -2851,7 +2845,7 @@
       </c>
       <c r="J46" s="40"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>90</v>
       </c>
@@ -2881,7 +2875,7 @@
       </c>
       <c r="J47" s="40"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>123</v>
       </c>
@@ -2911,7 +2905,7 @@
       </c>
       <c r="J48" s="40"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
         <v>124</v>
       </c>
@@ -2939,7 +2933,7 @@
       </c>
       <c r="J49" s="40"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="47" t="s">
         <v>91</v>
       </c>
@@ -2952,7 +2946,7 @@
       <c r="H50" s="54"/>
       <c r="I50" s="41"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>92</v>
       </c>
@@ -2977,7 +2971,7 @@
       <c r="H51" s="41"/>
       <c r="I51" s="41"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>93</v>
       </c>
@@ -3005,7 +2999,7 @@
       <c r="K52" s="34"/>
       <c r="L52" s="17"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>94</v>
       </c>
@@ -3033,7 +3027,7 @@
       <c r="K53" s="19"/>
       <c r="L53" s="17"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>127</v>
       </c>
@@ -3061,7 +3055,7 @@
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>96</v>
       </c>
@@ -3086,7 +3080,7 @@
       <c r="H55" s="41"/>
       <c r="I55" s="41"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>97</v>
       </c>
@@ -3111,7 +3105,7 @@
       <c r="H56" s="41"/>
       <c r="I56" s="41"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>99</v>
       </c>
@@ -3136,22 +3130,22 @@
       <c r="H57" s="41"/>
       <c r="I57" s="41"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="16"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="16"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="16"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="16"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="16"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="16"/>
     </row>
   </sheetData>
@@ -3163,25 +3157,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>128</v>
@@ -3190,7 +3184,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -3203,7 +3197,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
@@ -3216,7 +3210,7 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>136</v>
       </c>
@@ -3229,7 +3223,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>137</v>
       </c>
@@ -3242,7 +3236,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -3255,7 +3249,7 @@
         <v>0.4027</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -3268,7 +3262,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -3281,7 +3275,7 @@
         <v>0.3624</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>130</v>
       </c>
@@ -3294,7 +3288,7 @@
         <v>7446</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -3307,7 +3301,7 @@
         <v>2.6984304000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -3320,14 +3314,14 @@
         <v>872.06251456402208</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>128</v>
@@ -3336,7 +3330,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>131</v>
       </c>
@@ -3349,7 +3343,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>132</v>
       </c>
@@ -3362,7 +3356,7 @@
         <v>3.6999999999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>130</v>
       </c>
@@ -3375,7 +3369,7 @@
         <v>7446</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>146</v>
       </c>
@@ -3388,7 +3382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -3401,14 +3395,14 @@
         <v>30.956701347568568</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>128</v>
       </c>
@@ -3416,7 +3410,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>133</v>
       </c>
@@ -3429,7 +3423,7 @@
         <v>1.2599999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>134</v>
       </c>
@@ -3440,7 +3434,7 @@
         <v>947.8134</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>130</v>
       </c>
@@ -3453,7 +3447,7 @@
         <v>7446</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -3482,18 +3476,18 @@
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3502,7 +3496,7 @@
         <v>786.29928786524772</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3527,18 +3521,18 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3547,7 +3541,7 @@
         <v>15.162350502264802</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3569,21 +3563,21 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="42.5" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3592,7 +3586,7 @@
         <v>2241671.5347316861</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>

</xml_diff>